<commit_message>
Created the project files. Changed RC car SA and some requirements.
</commit_message>
<xml_diff>
--- a/Documents/Requirements.xlsx
+++ b/Documents/Requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghost\Desktop\GN\RC_Car_Git\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B473D5-C0CB-401A-A5B2-F760FBD7D3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6816BB3-533C-4BAD-8524-4EE40461D1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A5A1C29-1584-48CE-A1C7-67B9BDCE9B41}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Requirement number</t>
   </si>
@@ -185,15 +177,6 @@
     <t>It should be able to use the ESP camera module and send pictures using WiFi.</t>
   </si>
   <si>
-    <t>It should have a PID controller for controling the speed.</t>
-  </si>
-  <si>
-    <t>It should be able to switch between the two modes of operation: 1.The glove. 2.The Android App.</t>
-  </si>
-  <si>
-    <t>There isn't any priority between the 2 modes.</t>
-  </si>
-  <si>
     <t>It needs to receive an "analog" command, for example a command can be other than just go forward, go backward, it can be a percentage.</t>
   </si>
   <si>
@@ -213,9 +196,6 @@
   </si>
   <si>
     <t>Example of the 3rd byte: 127 is camera looking forward. 0 is camera looking left 90deg, 255 is camera looking right 90deg.</t>
-  </si>
-  <si>
-    <t>The car has a toggle button based on that the state will be changed.</t>
   </si>
 </sst>
 </file>
@@ -934,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0456E6-5D93-45E2-9006-75206BD13683}">
   <dimension ref="A1:Q183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1138,9 +1118,7 @@
       <c r="B8" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
@@ -1156,22 +1134,16 @@
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
     </row>
-    <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
@@ -1193,7 +1165,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1218,17 +1190,17 @@
         <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="3"/>
@@ -1249,10 +1221,10 @@
         <v>42</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>

</xml_diff>